<commit_message>
Prediction improved with additional descriptors and changed to predicting PCE instead of ranking methodology
</commit_message>
<xml_diff>
--- a/dyes_experimental_dataset.xlsx
+++ b/dyes_experimental_dataset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Dye</t>
   </si>
@@ -36,9 +36,6 @@
     <t>21a</t>
   </si>
   <si>
-    <t>Beetroot</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -66,18 +63,6 @@
     <t>Rutin</t>
   </si>
   <si>
-    <t>T1-simp</t>
-  </si>
-  <si>
-    <t>T2-simp</t>
-  </si>
-  <si>
-    <t>T3-simp</t>
-  </si>
-  <si>
-    <t>T4-simp</t>
-  </si>
-  <si>
     <t>expPCE</t>
   </si>
   <si>
@@ -88,6 +73,18 @@
   </si>
   <si>
     <t>expFF</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T1</t>
   </si>
 </sst>
 </file>
@@ -444,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,16 +459,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -547,7 +544,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>1.2999999999999999E-2</v>
+        <v>3.04E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6.28</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -555,13 +561,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>3.04E-2</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="C7" s="4">
-        <v>0.71199999999999997</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="D7" s="4">
-        <v>6.28</v>
+        <v>7.07</v>
       </c>
       <c r="E7" s="4">
         <v>0.68</v>
@@ -571,16 +577,16 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>3.4599999999999999E-2</v>
+      <c r="B8" s="3">
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="C8" s="4">
-        <v>0.71799999999999997</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="D8" s="4">
-        <v>7.07</v>
-      </c>
-      <c r="E8" s="4">
+        <v>5.09</v>
+      </c>
+      <c r="E8">
         <v>0.68</v>
       </c>
     </row>
@@ -589,16 +595,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>2.4899999999999999E-2</v>
+        <v>3.4099999999999998E-2</v>
       </c>
       <c r="C9" s="4">
-        <v>0.71699999999999997</v>
+        <v>0.76</v>
       </c>
       <c r="D9" s="4">
-        <v>5.09</v>
-      </c>
-      <c r="E9">
-        <v>0.68</v>
+        <v>10.42</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -606,50 +612,50 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>3.4099999999999998E-2</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="C10" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10.64</v>
+      </c>
+      <c r="E10" s="4">
         <v>0.76</v>
-      </c>
-      <c r="D10" s="4">
-        <v>10.42</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>3.7100000000000001E-2</v>
+      <c r="B11" s="6">
+        <v>5.5300000000000002E-2</v>
       </c>
       <c r="C11" s="4">
-        <v>0.85</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="D11" s="4">
-        <v>10.64</v>
+        <v>13.35</v>
       </c>
       <c r="E11" s="4">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
-        <v>5.5300000000000002E-2</v>
+      <c r="B12" s="7">
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="C12" s="4">
-        <v>0.66900000000000004</v>
+        <v>0.628</v>
       </c>
       <c r="D12" s="4">
-        <v>13.35</v>
+        <v>8.09</v>
       </c>
       <c r="E12" s="4">
-        <v>0.62</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -657,16 +663,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>3.4599999999999999E-2</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="C13" s="4">
-        <v>0.628</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="D13" s="4">
-        <v>8.09</v>
+        <v>5.48</v>
       </c>
       <c r="E13" s="4">
-        <v>0.68</v>
+        <v>0.67400000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -674,100 +680,83 @@
         <v>13</v>
       </c>
       <c r="B14" s="7">
-        <v>2.1499999999999998E-2</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="C14" s="4">
-        <v>0.58199999999999996</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D14" s="4">
-        <v>5.48</v>
+        <v>1.8260000000000001</v>
       </c>
       <c r="E14" s="4">
-        <v>0.67400000000000004</v>
+        <v>0.71299999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" s="7">
-        <v>7.1000000000000004E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="C15" s="4">
-        <v>0.54700000000000004</v>
+        <v>0.47</v>
       </c>
       <c r="D15" s="4">
-        <v>1.8260000000000001</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="E15" s="4">
-        <v>0.71299999999999997</v>
+        <v>0.50900000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7">
-        <v>5.4000000000000003E-3</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.1899999999999999E-2</v>
       </c>
       <c r="C16" s="4">
-        <v>0.47</v>
+        <v>0.51</v>
       </c>
       <c r="D16" s="4">
-        <v>2.2599999999999998</v>
+        <v>3.64</v>
       </c>
       <c r="E16" s="4">
-        <v>0.50900000000000001</v>
+        <v>0.64500000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" s="8">
-        <v>1.1899999999999999E-2</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="C17" s="4">
-        <v>0.51</v>
+        <v>0.45</v>
       </c>
       <c r="D17" s="4">
-        <v>3.64</v>
+        <v>0.64</v>
       </c>
       <c r="E17" s="4">
-        <v>0.64500000000000002</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8">
-        <v>2.2000000000000001E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="C18" s="4">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="D18" s="4">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="E18" s="4">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.48</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.66</v>
-      </c>
-      <c r="E19" s="4">
         <v>0.75</v>
       </c>
     </row>

</xml_diff>